<commit_message>
Cambios del 12/11/2018 (Reparado consumo excesivo RAM RMSE)
</commit_message>
<xml_diff>
--- a/docs/12_11_2018/HistogramaFotosUser.xlsx
+++ b/docs/12_11_2018/HistogramaFotosUser.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pp_1_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pp_1_\DOCUME~1\MobaXterm\slash\RemoteFiles\132290_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5E06A2-6349-4EE7-9652-B570A48FE954}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C110BBA7-C89B-4377-BA45-AFDB759C025F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13965" xr2:uid="{E4828925-D9D7-4ED8-A602-3E7DCCE51BD8}"/>
   </bookViews>
@@ -2072,7 +2072,7 @@
   <dimension ref="B1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>